<commit_message>
Add blacklist association to data files
</commit_message>
<xml_diff>
--- a/docs/data/questions/questions.xlsx
+++ b/docs/data/questions/questions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="460" windowWidth="27820" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="27820" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Quick?</t>
+  </si>
+  <si>
+    <t>tier</t>
   </si>
 </sst>
 </file>
@@ -446,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D32" sqref="D2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +467,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -475,8 +481,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>IF(A2&lt;10, 1, IF(A2&lt;100, 2, IF(A2&lt;10000, 3, 4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101</v>
       </c>
@@ -486,8 +496,12 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D32" si="0">IF(A3&lt;10, 1, IF(A3&lt;100, 2, IF(A3&lt;10000, 3, 4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>102</v>
       </c>
@@ -497,8 +511,12 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -508,8 +526,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>201</v>
       </c>
@@ -519,8 +541,12 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20101</v>
       </c>
@@ -530,8 +556,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2010101</v>
       </c>
@@ -541,8 +571,12 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20102</v>
       </c>
@@ -552,8 +586,12 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2010201</v>
       </c>
@@ -563,8 +601,12 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20103</v>
       </c>
@@ -574,8 +616,12 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20104</v>
       </c>
@@ -585,8 +631,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>202</v>
       </c>
@@ -596,8 +646,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20201</v>
       </c>
@@ -607,8 +661,12 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20203</v>
       </c>
@@ -618,8 +676,12 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -629,8 +691,12 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>301</v>
       </c>
@@ -640,8 +706,12 @@
       <c r="C17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>302</v>
       </c>
@@ -651,8 +721,12 @@
       <c r="C18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -662,8 +736,12 @@
       <c r="C19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -673,8 +751,12 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -684,8 +766,12 @@
       <c r="C21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -695,8 +781,12 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -706,8 +796,12 @@
       <c r="C23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>9</v>
       </c>
@@ -717,8 +811,12 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>901</v>
       </c>
@@ -728,8 +826,12 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>902</v>
       </c>
@@ -739,8 +841,12 @@
       <c r="C26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10</v>
       </c>
@@ -750,8 +856,12 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1001</v>
       </c>
@@ -761,8 +871,12 @@
       <c r="C28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -772,8 +886,12 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -783,8 +901,12 @@
       <c r="C30" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -794,8 +916,12 @@
       <c r="C31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>14</v>
       </c>
@@ -804,6 +930,10 @@
       </c>
       <c r="C32" t="s">
         <v>7</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>